<commit_message>
Adjustments for kidney test dataset
</commit_message>
<xml_diff>
--- a/test_datasets/Human_Kidney/test_annotation_kidney.xlsx
+++ b/test_datasets/Human_Kidney/test_annotation_kidney.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cauleyes/CPTR/DSP_Analysis/test_datasets/Human_Kidney/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14C009B8-FAF2-4B44-A3EA-C900C3ECFE7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71AFF64B-3DE1-5B4A-8A29-9F96AAC075C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1960" yWindow="1960" windowWidth="20440" windowHeight="11380" xr2:uid="{776D697D-50BF-449B-A436-D86E0F27716D}"/>
   </bookViews>
@@ -834,28 +834,35 @@
     <t>nuclei</t>
   </si>
   <si>
-    <t>PanCK-</t>
-  </si>
-  <si>
-    <t>PanCK--aoi-001</t>
-  </si>
-  <si>
-    <t>PanCK+</t>
-  </si>
-  <si>
-    <t>PanCK+-aoi-001</t>
-  </si>
-  <si>
     <t>slide name</t>
+  </si>
+  <si>
+    <t>PanCK_neg</t>
+  </si>
+  <si>
+    <t>PanCK_neg-aoi-001</t>
+  </si>
+  <si>
+    <t>PanCK_pos</t>
+  </si>
+  <si>
+    <t>PanCK_pos-aoi-001</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -902,12 +909,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -1225,14 +1233,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91D2ABA0-3808-4F97-A08C-4FABCCAEED45}">
   <dimension ref="A1:K240"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="28.83203125" customWidth="1"/>
     <col min="3" max="3" width="17.1640625" customWidth="1"/>
+    <col min="6" max="6" width="47.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -1243,7 +1252,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -2951,10 +2960,10 @@
         <v>1</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="H50" s="1">
         <v>23053.27</v>
@@ -2985,11 +2994,11 @@
       <c r="E51" s="1">
         <v>1</v>
       </c>
-      <c r="F51" s="1" t="s">
-        <v>266</v>
+      <c r="F51" s="4" t="s">
+        <v>267</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="H51" s="1">
         <v>137927.28</v>
@@ -3021,10 +3030,10 @@
         <v>2</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="H52" s="1">
         <v>17553.53</v>
@@ -3056,10 +3065,10 @@
         <v>2</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="H53" s="1">
         <v>123467.45</v>
@@ -3091,10 +3100,10 @@
         <v>3</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="H54" s="1">
         <v>22011.87</v>
@@ -3126,10 +3135,10 @@
         <v>3</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="H55" s="1">
         <v>209925.63</v>
@@ -3161,10 +3170,10 @@
         <v>4</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="H56" s="1">
         <v>17157.169999999998</v>
@@ -3196,10 +3205,10 @@
         <v>4</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="H57" s="1">
         <v>145616.81</v>
@@ -3231,10 +3240,10 @@
         <v>5</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="H58" s="1">
         <v>10254.219999999999</v>
@@ -3266,10 +3275,10 @@
         <v>5</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="H59" s="1">
         <v>105417.67</v>
@@ -3301,10 +3310,10 @@
         <v>6</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="H60" s="1">
         <v>34076.47</v>
@@ -3336,10 +3345,10 @@
         <v>6</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="H61" s="1">
         <v>137743.29999999999</v>
@@ -3810,10 +3819,10 @@
         <v>1</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="G75" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="H75" s="1">
         <v>20265.55</v>
@@ -3845,10 +3854,10 @@
         <v>1</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="H76" s="1">
         <v>91483.62</v>
@@ -3880,10 +3889,10 @@
         <v>2</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="G77" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="H77" s="1">
         <v>12966.08</v>
@@ -3915,10 +3924,10 @@
         <v>2</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="G78" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="H78" s="1">
         <v>133866.42000000001</v>
@@ -3950,10 +3959,10 @@
         <v>3</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="G79" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="H79" s="1">
         <v>23336.81</v>
@@ -3985,10 +3994,10 @@
         <v>3</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="G80" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="H80" s="1">
         <v>174741.6</v>
@@ -4020,10 +4029,10 @@
         <v>4</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="G81" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="H81" s="1">
         <v>15875.8</v>
@@ -4055,10 +4064,10 @@
         <v>4</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="G82" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="H82" s="1">
         <v>122888.57</v>
@@ -4090,10 +4099,10 @@
         <v>5</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="G83" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="H83" s="1">
         <v>23311.32</v>
@@ -4125,10 +4134,10 @@
         <v>5</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="G84" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="H84" s="1">
         <v>89287.05</v>
@@ -4160,10 +4169,10 @@
         <v>6</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="G85" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="H85" s="1">
         <v>9671.7900000000009</v>
@@ -4195,10 +4204,10 @@
         <v>6</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="G86" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="H86" s="1">
         <v>77969.649999999994</v>
@@ -5875,10 +5884,10 @@
         <v>1</v>
       </c>
       <c r="F134" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="G134" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="H134" s="1">
         <v>16012.17</v>
@@ -5910,10 +5919,10 @@
         <v>1</v>
       </c>
       <c r="F135" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="G135" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="H135" s="1">
         <v>127197.96</v>
@@ -5945,10 +5954,10 @@
         <v>2</v>
       </c>
       <c r="F136" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="G136" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="H136" s="1">
         <v>24168.74</v>
@@ -5980,10 +5989,10 @@
         <v>2</v>
       </c>
       <c r="F137" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="G137" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="H137" s="1">
         <v>71727.710000000006</v>
@@ -6015,10 +6024,10 @@
         <v>3</v>
       </c>
       <c r="F138" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="G138" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="H138" s="1">
         <v>34576.910000000003</v>
@@ -6050,10 +6059,10 @@
         <v>3</v>
       </c>
       <c r="F139" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="G139" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="H139" s="1">
         <v>91677.759999999995</v>
@@ -6085,10 +6094,10 @@
         <v>4</v>
       </c>
       <c r="F140" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="G140" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="H140" s="1">
         <v>29351.52</v>
@@ -6120,10 +6129,10 @@
         <v>4</v>
       </c>
       <c r="F141" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="G141" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="H141" s="1">
         <v>85295.1</v>
@@ -6155,10 +6164,10 @@
         <v>5</v>
       </c>
       <c r="F142" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="G142" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="H142" s="1">
         <v>12287.31</v>
@@ -6190,10 +6199,10 @@
         <v>5</v>
       </c>
       <c r="F143" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="G143" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="H143" s="1">
         <v>90680.26</v>
@@ -6225,10 +6234,10 @@
         <v>6</v>
       </c>
       <c r="F144" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="G144" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="H144" s="1">
         <v>19644.72</v>
@@ -6260,10 +6269,10 @@
         <v>6</v>
       </c>
       <c r="F145" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="G145" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="H145" s="1">
         <v>56847.48</v>
@@ -6680,10 +6689,10 @@
         <v>1</v>
       </c>
       <c r="F157" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="G157" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="H157" s="1">
         <v>22152.11</v>
@@ -6715,10 +6724,10 @@
         <v>1</v>
       </c>
       <c r="F158" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="G158" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="H158" s="1">
         <v>71817.919999999998</v>
@@ -6750,10 +6759,10 @@
         <v>2</v>
       </c>
       <c r="F159" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="G159" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="H159" s="1">
         <v>37316.699999999997</v>
@@ -6785,10 +6794,10 @@
         <v>2</v>
       </c>
       <c r="F160" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="G160" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="H160" s="1">
         <v>102112.73</v>
@@ -6820,10 +6829,10 @@
         <v>3</v>
       </c>
       <c r="F161" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="G161" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="H161" s="1">
         <v>18398.689999999999</v>
@@ -6855,10 +6864,10 @@
         <v>3</v>
       </c>
       <c r="F162" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="G162" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="H162" s="1">
         <v>85148.24</v>
@@ -6890,10 +6899,10 @@
         <v>4</v>
       </c>
       <c r="F163" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="G163" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="H163" s="1">
         <v>34778.480000000003</v>
@@ -6925,10 +6934,10 @@
         <v>4</v>
       </c>
       <c r="F164" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="G164" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="H164" s="1">
         <v>87237.5</v>
@@ -6960,10 +6969,10 @@
         <v>5</v>
       </c>
       <c r="F165" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="G165" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="H165" s="1">
         <v>23435.74</v>
@@ -6995,10 +7004,10 @@
         <v>5</v>
       </c>
       <c r="F166" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="G166" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="H166" s="1">
         <v>78840.789999999994</v>
@@ -7030,10 +7039,10 @@
         <v>6</v>
       </c>
       <c r="F167" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="G167" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="H167" s="1">
         <v>25414.45</v>
@@ -7065,10 +7074,10 @@
         <v>6</v>
       </c>
       <c r="F168" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="G168" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="H168" s="1">
         <v>102140.65</v>
@@ -7469,10 +7478,10 @@
         <v>6</v>
       </c>
       <c r="F180" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="G180" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="H180" s="1">
         <v>11634.61</v>
@@ -7504,10 +7513,10 @@
         <v>6</v>
       </c>
       <c r="F181" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="G181" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="H181" s="1">
         <v>74251.72</v>
@@ -7539,10 +7548,10 @@
         <v>7</v>
       </c>
       <c r="F182" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="G182" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="H182" s="1">
         <v>17370.78</v>
@@ -7574,10 +7583,10 @@
         <v>7</v>
       </c>
       <c r="F183" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="G183" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="H183" s="1">
         <v>81639.25</v>
@@ -7609,10 +7618,10 @@
         <v>8</v>
       </c>
       <c r="F184" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="G184" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="H184" s="1">
         <v>10375.91</v>
@@ -7644,10 +7653,10 @@
         <v>8</v>
       </c>
       <c r="F185" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="G185" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="H185" s="1">
         <v>73735.649999999994</v>
@@ -7679,10 +7688,10 @@
         <v>9</v>
       </c>
       <c r="F186" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="G186" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="H186" s="1">
         <v>6450.01</v>
@@ -7714,10 +7723,10 @@
         <v>9</v>
       </c>
       <c r="F187" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="G187" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="H187" s="1">
         <v>68227.62</v>
@@ -7749,10 +7758,10 @@
         <v>10</v>
       </c>
       <c r="F188" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="G188" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="H188" s="1">
         <v>12227.75</v>
@@ -7784,10 +7793,10 @@
         <v>10</v>
       </c>
       <c r="F189" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="G189" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="H189" s="1">
         <v>78998.740000000005</v>
@@ -7819,10 +7828,10 @@
         <v>11</v>
       </c>
       <c r="F190" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="G190" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="H190" s="1">
         <v>10457.450000000001</v>
@@ -7854,10 +7863,10 @@
         <v>11</v>
       </c>
       <c r="F191" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="G191" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="H191" s="1">
         <v>46423.18</v>
@@ -8328,10 +8337,10 @@
         <v>7</v>
       </c>
       <c r="F205" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="G205" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="H205" s="1">
         <v>8313.84</v>
@@ -8363,10 +8372,10 @@
         <v>7</v>
       </c>
       <c r="F206" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="G206" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="H206" s="1">
         <v>96174.64</v>
@@ -8398,10 +8407,10 @@
         <v>8</v>
       </c>
       <c r="F207" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="G207" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="H207" s="1">
         <v>6364.16</v>
@@ -8433,10 +8442,10 @@
         <v>8</v>
       </c>
       <c r="F208" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="G208" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="H208" s="1">
         <v>60662.64</v>
@@ -8468,10 +8477,10 @@
         <v>9</v>
       </c>
       <c r="F209" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="G209" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="H209" s="1">
         <v>21252.87</v>
@@ -8503,10 +8512,10 @@
         <v>9</v>
       </c>
       <c r="F210" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="G210" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="H210" s="1">
         <v>85405.91</v>
@@ -8538,10 +8547,10 @@
         <v>10</v>
       </c>
       <c r="F211" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="G211" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="H211" s="1">
         <v>7349.79</v>
@@ -8573,10 +8582,10 @@
         <v>10</v>
       </c>
       <c r="F212" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="G212" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="H212" s="1">
         <v>66892.02</v>
@@ -8608,10 +8617,10 @@
         <v>11</v>
       </c>
       <c r="F213" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="G213" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="H213" s="1">
         <v>11468.34</v>
@@ -8643,10 +8652,10 @@
         <v>11</v>
       </c>
       <c r="F214" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="G214" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="H214" s="1">
         <v>118494.68</v>
@@ -8678,10 +8687,10 @@
         <v>12</v>
       </c>
       <c r="F215" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="G215" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="H215" s="1">
         <v>12457.97</v>
@@ -8713,10 +8722,10 @@
         <v>12</v>
       </c>
       <c r="F216" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="G216" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="H216" s="1">
         <v>160617.85</v>
@@ -9098,10 +9107,10 @@
         <v>7</v>
       </c>
       <c r="F227" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="G227" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="H227" s="1">
         <v>11510.39</v>
@@ -9133,10 +9142,10 @@
         <v>7</v>
       </c>
       <c r="F228" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="G228" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="H228" s="1">
         <v>61035.47</v>
@@ -9168,10 +9177,10 @@
         <v>8</v>
       </c>
       <c r="F229" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="G229" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="H229" s="1">
         <v>10672.48</v>
@@ -9203,10 +9212,10 @@
         <v>8</v>
       </c>
       <c r="F230" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="G230" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="H230" s="1">
         <v>70102.8</v>
@@ -9238,10 +9247,10 @@
         <v>9</v>
       </c>
       <c r="F231" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="G231" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="H231" s="1">
         <v>15331.41</v>
@@ -9273,10 +9282,10 @@
         <v>9</v>
       </c>
       <c r="F232" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="G232" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="H232" s="1">
         <v>120199.59</v>
@@ -9308,10 +9317,10 @@
         <v>10</v>
       </c>
       <c r="F233" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="G233" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="H233" s="1">
         <v>24825.61</v>
@@ -9343,10 +9352,10 @@
         <v>10</v>
       </c>
       <c r="F234" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="G234" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="H234" s="1">
         <v>184639.44</v>
@@ -9378,10 +9387,10 @@
         <v>11</v>
       </c>
       <c r="F235" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="G235" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="H235" s="1">
         <v>8595.7000000000007</v>
@@ -9413,10 +9422,10 @@
         <v>11</v>
       </c>
       <c r="F236" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="G236" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="H236" s="1">
         <v>67263.41</v>
@@ -9448,10 +9457,10 @@
         <v>12</v>
       </c>
       <c r="F237" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="G237" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="H237" s="1">
         <v>9549.2000000000007</v>
@@ -9483,10 +9492,10 @@
         <v>12</v>
       </c>
       <c r="F238" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="G238" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="H238" s="1">
         <v>67032.55</v>

</xml_diff>